<commit_message>
added rare candy chance to the spresheet
</commit_message>
<xml_diff>
--- a/Project1/Non-coding/Prob&Stats cardmulligan.xlsx
+++ b/Project1/Non-coding/Prob&Stats cardmulligan.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PokEm\Desktop\School Folders\Prob &amp; Stats\Project1\Non-coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B501BF20-3336-4EAA-9990-134B55AB6B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52CCFF2-7B7E-45E2-8F21-8E5E11002905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{D085B485-A8D0-4383-8CAD-33BD3269913A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Card Mulligan" sheetId="1" r:id="rId1"/>
+    <sheet name="Rare Candy" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -159,7 +159,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>'Card Mulligan'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -207,7 +207,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$61</c:f>
+              <c:f>'Card Mulligan'!$A$2:$A$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="60"/>
@@ -396,7 +396,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$61</c:f>
+              <c:f>'Card Mulligan'!$B$2:$B$61</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="60"/>
@@ -777,7 +777,373 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Rare Candy'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>brick percent</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Rare Candy'!$A$2:$A$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Rare Candy'!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.6400000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5200000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.6199999999999995E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-042A-4A10-AC1C-3B642CC7DE57}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1207031680"/>
+        <c:axId val="1091820032"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1207031680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1091820032"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1091820032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1207031680"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1333,6 +1699,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1354,6 +2223,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBB221C8-A82A-28F3-8FBC-3C4379ADD007}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{766C205C-CE3A-2CA6-2C89-D88442303A45}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2201,7 +3111,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2222,23 +3132,36 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" s="1">
+        <v>1.6400000000000001E-2</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" s="1">
+        <v>3.5200000000000002E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" s="1">
+        <v>4.8500000000000001E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" s="1">
+        <v>6.6199999999999995E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>